<commit_message>
testes exoticos da tropa do rei sapo
</commit_message>
<xml_diff>
--- a/rascunhos/PLANEJAMENTO DE REGRAS.xlsx
+++ b/rascunhos/PLANEJAMENTO DE REGRAS.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ifscedubr-my.sharepoint.com/personal/bernardo_mm05_aluno_ifsc_edu_br/Documents/Faculdade/5ª Fase/Inteligência Artificial/nocapIA_PythonVersion/rascunhos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C839DD62-C924-4844-B9FB-E8CAB6CB22A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C839DD62-C924-4844-B9FB-E8CAB6CB22A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{F6489F90-9959-4FC0-B5E4-378F8586A803}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09682E15-2537-4E7D-9D23-4AB65F69A6DB}"/>
+    <workbookView xWindow="-10785" yWindow="2295" windowWidth="21600" windowHeight="11325" xr2:uid="{09682E15-2537-4E7D-9D23-4AB65F69A6DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$I$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$2:$I$46</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="120">
   <si>
     <t>problemas</t>
   </si>
@@ -378,17 +378,23 @@
     <t>review function</t>
   </si>
   <si>
-    <t xml:space="preserve">tela preta= </t>
-  </si>
-  <si>
     <t>Pergunta</t>
+  </si>
+  <si>
+    <t>CAMADA R-&gt;</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,8 +410,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +531,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CACC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -674,58 +694,30 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDEBF7"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FF66CACC"/>
       <color rgb="FFFF6600"/>
       <color rgb="FF33CCFF"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FFFFFF66"/>
-      <color rgb="FFFF5050"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1036,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171F910A-E316-4DF9-A7AE-C7737AB75AA4}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,94 +1046,88 @@
     <col min="9" max="9" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="3" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="31"/>
+      <c r="E3" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="23"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
+    <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="23"/>
+        <v>37</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1159,7 +1145,9 @@
       <c r="D5" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="26" t="s">
+        <v>115</v>
+      </c>
       <c r="F5" s="25"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1222,15 +1210,15 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>103</v>
@@ -1243,15 +1231,15 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>103</v>
@@ -1262,15 +1250,15 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>103</v>
@@ -1281,95 +1269,95 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="24"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>29</v>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>21</v>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="23"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>43</v>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="23"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>109</v>
@@ -1380,95 +1368,93 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="27"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="25"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="24"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>21</v>
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="23"/>
+        <v>34</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="25"/>
+      <c r="E20" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="23"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>111</v>
@@ -1479,15 +1465,15 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>111</v>
@@ -1498,74 +1484,74 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="24"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="25"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>29</v>
+    <row r="24" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="23"/>
+        <v>77</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="27"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="25"/>
+      <c r="E25" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="23"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>108</v>
@@ -1576,15 +1562,15 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>108</v>
@@ -1595,15 +1581,15 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>108</v>
@@ -1614,74 +1600,74 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="24"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>21</v>
+    <row r="30" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="23"/>
+        <v>92</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="27"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="25"/>
+      <c r="E31" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="23"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>105</v>
@@ -1692,15 +1678,15 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>105</v>
@@ -1711,74 +1697,74 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="24"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>12</v>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F35" s="23"/>
+        <v>42</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E35" s="27"/>
+      <c r="F35" s="24"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="23"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>21</v>
+    <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>104</v>
@@ -1789,15 +1775,15 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>44</v>
+    <row r="38" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>104</v>
@@ -1808,15 +1794,15 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>104</v>
@@ -1827,15 +1813,15 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>104</v>
@@ -1846,131 +1832,153 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="24"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="25"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>21</v>
+    <row r="42" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F42" s="23"/>
+        <v>101</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="27"/>
+      <c r="F42" s="24"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="24"/>
+      <c r="E43" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="23"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+    <row r="44" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="27"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B45" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C45" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12" t="s">
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12" t="s">
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B46" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C46" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11" t="s">
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11" t="s">
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I45" xr:uid="{784ED9ED-1E32-4200-8F48-31F2C25C4B24}">
-    <sortState ref="A2:I45">
-      <sortCondition descending="1" ref="D1:D45"/>
+  <autoFilter ref="A2:I46" xr:uid="{784ED9ED-1E32-4200-8F48-31F2C25C4B24}">
+    <sortState ref="A3:I46">
+      <sortCondition descending="1" ref="D2:D46"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="17">
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E35:E41"/>
-    <mergeCell ref="E30:E34"/>
-    <mergeCell ref="E24:E29"/>
-    <mergeCell ref="E19:E23"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="F35:F41"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="F19:F23"/>
-    <mergeCell ref="F24:F29"/>
+  <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F9:F13"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="E36:E42"/>
+    <mergeCell ref="E31:E35"/>
+    <mergeCell ref="E25:E30"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="F31:F35"/>
+    <mergeCell ref="F36:F42"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="F25:F30"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>